<commit_message>
edit py to excel by using soal 1 func
</commit_message>
<xml_diff>
--- a/Rico Putra Pradana/Soal_4/rico_putra_pradana.xlsx
+++ b/Rico Putra Pradana/Soal_4/rico_putra_pradana.xlsx
@@ -25,13 +25,13 @@
     <t>usia</t>
   </si>
   <si>
-    <t>rico</t>
+    <t>Rico</t>
   </si>
   <si>
     <t>rico.putra@outlook.co.id</t>
   </si>
   <si>
-    <t>22 Tahun</t>
+    <t>22 Tahun 7 Bulan</t>
   </si>
 </sst>
 </file>
@@ -370,7 +370,7 @@
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="25.7109375" customWidth="1"/>
-    <col min="3" max="3" width="9.7109375" customWidth="1"/>
+    <col min="3" max="3" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>

<commit_message>
DONE add explanation for soal 4
</commit_message>
<xml_diff>
--- a/Rico Putra Pradana/Soal_4/rico_putra_pradana.xlsx
+++ b/Rico Putra Pradana/Soal_4/rico_putra_pradana.xlsx
@@ -25,13 +25,13 @@
     <t>usia</t>
   </si>
   <si>
-    <t>Mukidi</t>
-  </si>
-  <si>
-    <t>mukidi@ai.astra.co.id</t>
-  </si>
-  <si>
-    <t>27 Tahun 9 Bulan</t>
+    <t>Rico Putra Pradana</t>
+  </si>
+  <si>
+    <t>rico.putra@outlook.co.id</t>
+  </si>
+  <si>
+    <t>22 Tahun 7 Bulan</t>
   </si>
 </sst>
 </file>
@@ -369,8 +369,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="19.7109375" customWidth="1"/>
+    <col min="2" max="2" width="25.7109375" customWidth="1"/>
     <col min="3" max="3" width="17.7109375" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>